<commit_message>
Mengisi file data induk penduduk
</commit_message>
<xml_diff>
--- a/PEMERINTAHAN/Data-Induk-Penduduk.xlsx
+++ b/PEMERINTAHAN/Data-Induk-Penduduk.xlsx
@@ -9,8 +9,22 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>ujang</t>
+  </si>
+  <si>
+    <t>imas</t>
+  </si>
+  <si>
+    <t>ari</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -130,7 +144,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -165,7 +178,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -342,12 +354,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mengisi asep ke file data induk penduduk
</commit_message>
<xml_diff>
--- a/PEMERINTAHAN/Data-Induk-Penduduk.xlsx
+++ b/PEMERINTAHAN/Data-Induk-Penduduk.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ujang</t>
   </si>
@@ -23,6 +23,18 @@
   </si>
   <si>
     <t>ari</t>
+  </si>
+  <si>
+    <t>asep</t>
+  </si>
+  <si>
+    <t>siti</t>
+  </si>
+  <si>
+    <t>aska</t>
+  </si>
+  <si>
+    <t>saka</t>
   </si>
 </sst>
 </file>
@@ -354,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -377,6 +389,26 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>